<commit_message>
Update 'Floorplan rules.xlsx' from the live Google Sheet
</commit_message>
<xml_diff>
--- a/Floorplan rules.xlsx
+++ b/Floorplan rules.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$A$1092</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$A$1089</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -33,37 +33,34 @@
 	-Ruth Elder</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B189">
+    <comment authorId="0" ref="B186">
       <text>
         <t xml:space="preserve">No items at this location
 	-Ruth Elder</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B188">
+    <comment authorId="0" ref="B185">
       <text>
         <t xml:space="preserve">No items at this location
 	-Ruth Elder</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B182">
+    <comment authorId="0" ref="B179">
       <text>
         <t xml:space="preserve">No items listed at this location
 	-Ruth Elder</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B178">
+    <comment authorId="0" ref="B176">
       <text>
         <t xml:space="preserve">Items still listed- wait for Sue E to complete work on checking
+	-Ruth Elder
+----
+Items still listed- wait for Sue E to complete work on checking
 	-Ruth Elder</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B177">
-      <text>
-        <t xml:space="preserve">Items still listed- wait for Sue E to complete work on checking
-	-Ruth Elder</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B175">
+    <comment authorId="0" ref="B174">
       <text>
         <t xml:space="preserve">No items at this location
 	-Ruth Elder
@@ -78,7 +75,7 @@
 	-Ruth Elder</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B174">
+    <comment authorId="0" ref="B173">
       <text>
         <t xml:space="preserve">No items at this location
 	-Ruth Elder
@@ -155,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="290">
   <si>
     <t>Library code</t>
   </si>
@@ -199,7 +196,7 @@
     <t>This item is located in the Green zone on Floor 1 of the JB Morrell Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/morrell_floor1.png</t>
+    <t>https://drive.google.com/uc?id=1zM2hoTBo_UH-TbXNskE13u04yv1lVQED</t>
   </si>
   <si>
     <t>POP</t>
@@ -233,7 +230,7 @@
     <t>This item is located in the Purple zone on Floor 2 of the JB Morrell Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/morrell_floor2.png</t>
+    <t>https://drive.google.com/uc?id=1WBdsGbnavzZI3wG6ugDzxqUXDL-nVzO2</t>
   </si>
   <si>
     <t>This item is located in the Purple zone on Floor 2 of the JB Morrell Library.
@@ -332,7 +329,7 @@
     <t>This item is located in Compact Store 2 on Floor 0 of the JB Morrell Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/morrell_floor0.png</t>
+    <t>https://drive.google.com/uc?id=1yDoVeWqld-FS89wXCx07xsszQtE1lfIE</t>
   </si>
   <si>
     <t>K</t>
@@ -389,7 +386,7 @@
     <t>This item is located in the John Paynter Music Library on Floor 0 of the Harry Fairhurst Building.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/fairhurst_floor0.png</t>
+    <t>https://drive.google.com/uc?id=1MCqnsTpvHgkn1uuuG0iF5ixWY9k607R7</t>
   </si>
   <si>
     <t>HFF</t>
@@ -478,7 +475,7 @@
     <t>This item is located on Floor 3 of the JB Morrell Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/morrell_floor3.png</t>
+    <t>https://drive.google.com/uc?id=1tx1Jzt42Q6kpxVTIbtJZQ0XWfyZekccL</t>
   </si>
   <si>
     <t>This item is located on Floor 3 of the JB Morrell Library.
@@ -883,7 +880,7 @@
     <t>This item is located on Floor 1 of the Harry Fairhurst Building.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/fairhurst_floor1.png</t>
+    <t>https://drive.google.com/uc?id=1_s0oD9ZwdVRY1geUDiOochDv_jkQmCnU</t>
   </si>
   <si>
     <t>RB</t>
@@ -898,7 +895,7 @@
     <t>This item is located in the Humanities Research Reading Room on Floor 1 of the Raymond Burton Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/burton_floor1.png</t>
+    <t>https://drive.google.com/uc?id=10b8kQ8zxJxnJSMGpPa1XaWqvRP9diXAv</t>
   </si>
   <si>
     <t>ELT</t>
@@ -907,12 +904,6 @@
     <t>Burton - Reading Room - Elton Collection</t>
   </si>
   <si>
-    <t>MFC</t>
-  </si>
-  <si>
-    <t>Burton - Reading Room - Microcard</t>
-  </si>
-  <si>
     <t>MFFC</t>
   </si>
   <si>
@@ -943,7 +934,7 @@
     <t>This item is located on the First Floor of the King's Manor Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/kings-manor-floor-1-2019.png</t>
+    <t>https://drive.google.com/uc?id=1lfOA-WPHAm59tciS2Z3dOvru2Joekzki</t>
   </si>
   <si>
     <t>KMF</t>
@@ -952,18 +943,6 @@
     <t>First floor - Folio</t>
   </si>
   <si>
-    <t>KMMFC</t>
-  </si>
-  <si>
-    <t>First floor - Microfiche</t>
-  </si>
-  <si>
-    <t>KMMFL</t>
-  </si>
-  <si>
-    <t>First floor - Microfilm</t>
-  </si>
-  <si>
     <t>KMPAM</t>
   </si>
   <si>
@@ -1006,7 +985,7 @@
     <t>This item is located on the Ground Floor of the King's Manor Library.</t>
   </si>
   <si>
-    <t>https://www.york.ac.uk/media/library/images/imagesforfloorplans/kings-manor-floor-0-2019.png</t>
+    <t>https://drive.google.com/uc?id=1zUXkER8Yb8J3Ghv3PSmQhyKFmbzLBilm</t>
   </si>
   <si>
     <t>KMAPA</t>
@@ -1036,31 +1015,28 @@
     <t>WO</t>
   </si>
   <si>
-    <t>Wormald Room</t>
-  </si>
-  <si>
-    <t>King's Manor Library Wormald Room</t>
+    <t>Wormald Collection</t>
+  </si>
+  <si>
+    <t>King's Manor Library Wormald Collection</t>
   </si>
   <si>
     <t>WOF</t>
   </si>
   <si>
-    <t>Wormald Room - Folio</t>
+    <t>Wormald Collection - Folio</t>
   </si>
   <si>
     <t>WOPA</t>
   </si>
   <si>
-    <t>Wormald Room - Pamphlet</t>
+    <t>Wormald Collection - Pamphlet</t>
   </si>
   <si>
     <t>WOQ</t>
   </si>
   <si>
-    <t>Wormald Room - Quarto</t>
-  </si>
-  <si>
-    <t>Last updated: 19.11.19  RE</t>
+    <t>Wormald Collection - Quarto</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1081,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,12 +1094,6 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -1131,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1186,9 +1156,6 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
@@ -1198,7 +1165,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -5717,7 +5684,7 @@
     </row>
     <row r="174">
       <c r="A174" s="3" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>251</v>
@@ -5728,40 +5695,40 @@
       <c r="D174" s="13"/>
       <c r="E174" s="14"/>
       <c r="F174" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="G174" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="H174" s="7" t="s">
-        <v>242</v>
+        <v>253</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H174" s="9" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D175" s="13"/>
       <c r="E175" s="14"/>
       <c r="F175" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G175" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H175" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="G175" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="H175" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>258</v>
@@ -5772,62 +5739,62 @@
       <c r="D176" s="13"/>
       <c r="E176" s="14"/>
       <c r="F176" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G176" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H176" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="G176" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H176" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C177" s="18" t="s">
+      <c r="C177" s="3" t="s">
         <v>261</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="14"/>
       <c r="F177" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G177" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H177" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="G177" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H177" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C178" s="18" t="s">
+      <c r="C178" s="3" t="s">
         <v>263</v>
       </c>
       <c r="D178" s="13"/>
       <c r="E178" s="14"/>
       <c r="F178" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G178" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H178" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="G178" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H178" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>264</v>
@@ -5838,18 +5805,18 @@
       <c r="D179" s="13"/>
       <c r="E179" s="14"/>
       <c r="F179" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G179" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H179" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="G179" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H179" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>266</v>
@@ -5860,106 +5827,106 @@
       <c r="D180" s="13"/>
       <c r="E180" s="14"/>
       <c r="F180" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G180" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H180" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="G180" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H180" s="7" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B181" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B181" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="C181" s="3" t="s">
+      <c r="C181" s="18" t="s">
         <v>269</v>
       </c>
       <c r="D181" s="13"/>
       <c r="E181" s="14"/>
       <c r="F181" s="3" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="G181" s="11" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="H181" s="7" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D182" s="13"/>
       <c r="E182" s="14"/>
       <c r="F182" s="3" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="G182" s="11" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="H182" s="7" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>273</v>
+        <v>251</v>
+      </c>
+      <c r="B183" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="C183" s="20" t="s">
+        <v>276</v>
       </c>
       <c r="D183" s="13"/>
       <c r="E183" s="14"/>
       <c r="F183" s="3" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="G183" s="11" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="H183" s="7" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B184" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="C184" s="19" t="s">
-        <v>275</v>
+        <v>277</v>
+      </c>
+      <c r="C184" s="18" t="s">
+        <v>278</v>
       </c>
       <c r="D184" s="13"/>
       <c r="E184" s="14"/>
       <c r="F184" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G184" s="11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H184" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>279</v>
@@ -5970,177 +5937,121 @@
       <c r="D185" s="13"/>
       <c r="E185" s="14"/>
       <c r="F185" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G185" s="11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H185" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B186" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B186" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C186" s="21" t="s">
+      <c r="C186" s="3" t="s">
         <v>282</v>
       </c>
       <c r="D186" s="13"/>
       <c r="E186" s="14"/>
       <c r="F186" s="3" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="G186" s="11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H186" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B187" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C187" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B187" s="3" t="s">
         <v>284</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="D187" s="13"/>
       <c r="E187" s="14"/>
       <c r="F187" s="3" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="G187" s="11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H187" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D188" s="13"/>
       <c r="E188" s="14"/>
       <c r="F188" s="3" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="G188" s="11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H188" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D189" s="13"/>
       <c r="E189" s="14"/>
       <c r="F189" s="3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="G189" s="11" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H189" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="D190" s="13"/>
       <c r="E190" s="14"/>
-      <c r="F190" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="G190" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="H190" s="7" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="191">
-      <c r="A191" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>293</v>
-      </c>
+      <c r="C191" s="21"/>
       <c r="D191" s="13"/>
       <c r="E191" s="14"/>
-      <c r="F191" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="G191" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="H191" s="7" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="192">
-      <c r="A192" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="D192" s="13"/>
       <c r="E192" s="14"/>
-      <c r="F192" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="G192" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="H192" s="7" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="193">
       <c r="D193" s="13"/>
       <c r="E193" s="14"/>
     </row>
     <row r="194">
-      <c r="C194" s="22" t="s">
-        <v>296</v>
-      </c>
       <c r="D194" s="13"/>
       <c r="E194" s="14"/>
     </row>
@@ -9724,20 +9635,8 @@
       <c r="D1089" s="13"/>
       <c r="E1089" s="14"/>
     </row>
-    <row r="1090">
-      <c r="D1090" s="13"/>
-      <c r="E1090" s="14"/>
-    </row>
-    <row r="1091">
-      <c r="D1091" s="13"/>
-      <c r="E1091" s="14"/>
-    </row>
-    <row r="1092">
-      <c r="D1092" s="13"/>
-      <c r="E1092" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$A$1092"/>
+  <autoFilter ref="$A$1:$A$1089"/>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="H2"/>
     <hyperlink r:id="rId3" ref="H3"/>
@@ -9927,11 +9826,8 @@
     <hyperlink r:id="rId187" ref="H187"/>
     <hyperlink r:id="rId188" ref="H188"/>
     <hyperlink r:id="rId189" ref="H189"/>
-    <hyperlink r:id="rId190" ref="H190"/>
-    <hyperlink r:id="rId191" ref="H191"/>
-    <hyperlink r:id="rId192" ref="H192"/>
   </hyperlinks>
-  <drawing r:id="rId193"/>
-  <legacyDrawing r:id="rId194"/>
+  <drawing r:id="rId190"/>
+  <legacyDrawing r:id="rId191"/>
 </worksheet>
 </file>
</xml_diff>